<commit_message>
fix float liczba stanowisk
</commit_message>
<xml_diff>
--- a/GCMDataBase.xlsx
+++ b/GCMDataBase.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3356" uniqueCount="1518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3390" uniqueCount="1518">
   <si>
     <t>domainName</t>
   </si>
@@ -16770,8 +16770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E191" sqref="E191"/>
+    <sheetView tabSelected="1" topLeftCell="E85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K138" sqref="K138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21055,11 +21055,17 @@
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="5"/>
-      <c r="F128" s="9"/>
+      <c r="F128" s="9">
+        <v>21</v>
+      </c>
       <c r="G128" s="9"/>
       <c r="H128" s="6"/>
-      <c r="I128" s="6"/>
-      <c r="J128" s="6"/>
+      <c r="I128" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J128" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
@@ -21073,11 +21079,17 @@
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="5"/>
-      <c r="F129" s="9"/>
+      <c r="F129" s="9">
+        <v>6</v>
+      </c>
       <c r="G129" s="9"/>
       <c r="H129" s="6"/>
-      <c r="I129" s="6"/>
-      <c r="J129" s="6"/>
+      <c r="I129" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J129" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
@@ -21091,11 +21103,17 @@
       </c>
       <c r="D130" s="9"/>
       <c r="E130" s="5"/>
-      <c r="F130" s="9"/>
+      <c r="F130" s="9">
+        <v>24</v>
+      </c>
       <c r="G130" s="9"/>
       <c r="H130" s="6"/>
-      <c r="I130" s="6"/>
-      <c r="J130" s="6"/>
+      <c r="I130" s="30" t="s">
+        <v>833</v>
+      </c>
+      <c r="J130" s="30" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
@@ -21109,11 +21127,17 @@
       </c>
       <c r="D131" s="9"/>
       <c r="E131" s="5"/>
-      <c r="F131" s="9"/>
+      <c r="F131" s="9">
+        <v>15</v>
+      </c>
       <c r="G131" s="9"/>
       <c r="H131" s="6"/>
-      <c r="I131" s="6"/>
-      <c r="J131" s="6"/>
+      <c r="I131" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J131" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
@@ -21127,11 +21151,17 @@
       </c>
       <c r="D132" s="9"/>
       <c r="E132" s="5"/>
-      <c r="F132" s="9"/>
+      <c r="F132" s="9">
+        <v>20</v>
+      </c>
       <c r="G132" s="9"/>
       <c r="H132" s="6"/>
-      <c r="I132" s="6"/>
-      <c r="J132" s="6"/>
+      <c r="I132" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J132" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
@@ -21145,11 +21175,17 @@
       </c>
       <c r="D133" s="9"/>
       <c r="E133" s="5"/>
-      <c r="F133" s="9"/>
+      <c r="F133" s="9">
+        <v>21</v>
+      </c>
       <c r="G133" s="9"/>
       <c r="H133" s="6"/>
-      <c r="I133" s="6"/>
-      <c r="J133" s="6"/>
+      <c r="I133" s="30" t="s">
+        <v>833</v>
+      </c>
+      <c r="J133" s="30" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
@@ -21163,11 +21199,17 @@
       </c>
       <c r="D134" s="9"/>
       <c r="E134" s="5"/>
-      <c r="F134" s="9"/>
+      <c r="F134" s="9">
+        <v>24</v>
+      </c>
       <c r="G134" s="9"/>
       <c r="H134" s="6"/>
-      <c r="I134" s="6"/>
-      <c r="J134" s="6"/>
+      <c r="I134" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J134" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
@@ -21181,11 +21223,17 @@
       </c>
       <c r="D135" s="9"/>
       <c r="E135" s="5"/>
-      <c r="F135" s="9"/>
+      <c r="F135" s="9">
+        <v>12</v>
+      </c>
       <c r="G135" s="9"/>
       <c r="H135" s="6"/>
-      <c r="I135" s="6"/>
-      <c r="J135" s="6"/>
+      <c r="I135" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J135" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
@@ -21199,11 +21247,17 @@
       </c>
       <c r="D136" s="9"/>
       <c r="E136" s="5"/>
-      <c r="F136" s="9"/>
+      <c r="F136" s="9">
+        <v>8</v>
+      </c>
       <c r="G136" s="9"/>
       <c r="H136" s="6"/>
-      <c r="I136" s="6"/>
-      <c r="J136" s="6"/>
+      <c r="I136" s="30" t="s">
+        <v>833</v>
+      </c>
+      <c r="J136" s="30" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
@@ -21217,11 +21271,17 @@
       </c>
       <c r="D137" s="9"/>
       <c r="E137" s="5"/>
-      <c r="F137" s="9"/>
+      <c r="F137" s="9">
+        <v>20</v>
+      </c>
       <c r="G137" s="9"/>
       <c r="H137" s="6"/>
-      <c r="I137" s="6"/>
-      <c r="J137" s="6"/>
+      <c r="I137" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J137" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
@@ -21235,11 +21295,17 @@
       </c>
       <c r="D138" s="9"/>
       <c r="E138" s="5"/>
-      <c r="F138" s="9"/>
+      <c r="F138" s="9">
+        <v>20</v>
+      </c>
       <c r="G138" s="9"/>
       <c r="H138" s="6"/>
-      <c r="I138" s="6"/>
-      <c r="J138" s="6"/>
+      <c r="I138" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J138" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
@@ -21253,11 +21319,17 @@
       </c>
       <c r="D139" s="9"/>
       <c r="E139" s="5"/>
-      <c r="F139" s="9"/>
+      <c r="F139" s="9">
+        <v>20</v>
+      </c>
       <c r="G139" s="9"/>
       <c r="H139" s="6"/>
-      <c r="I139" s="6"/>
-      <c r="J139" s="6"/>
+      <c r="I139" s="30" t="s">
+        <v>833</v>
+      </c>
+      <c r="J139" s="30" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
@@ -21271,11 +21343,17 @@
       </c>
       <c r="D140" s="9"/>
       <c r="E140" s="5"/>
-      <c r="F140" s="9"/>
+      <c r="F140" s="9">
+        <v>20</v>
+      </c>
       <c r="G140" s="9"/>
       <c r="H140" s="6"/>
-      <c r="I140" s="6"/>
-      <c r="J140" s="6"/>
+      <c r="I140" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J140" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141">
@@ -21289,11 +21367,17 @@
       </c>
       <c r="D141" s="9"/>
       <c r="E141" s="5"/>
-      <c r="F141" s="9"/>
+      <c r="F141" s="9">
+        <v>41</v>
+      </c>
       <c r="G141" s="9"/>
       <c r="H141" s="6"/>
-      <c r="I141" s="6"/>
-      <c r="J141" s="6"/>
+      <c r="I141" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J141" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
@@ -21307,11 +21391,17 @@
       </c>
       <c r="D142" s="9"/>
       <c r="E142" s="5"/>
-      <c r="F142" s="9"/>
+      <c r="F142" s="9">
+        <v>5</v>
+      </c>
       <c r="G142" s="9"/>
       <c r="H142" s="6"/>
-      <c r="I142" s="6"/>
-      <c r="J142" s="6"/>
+      <c r="I142" s="30" t="s">
+        <v>833</v>
+      </c>
+      <c r="J142" s="30" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
@@ -21325,11 +21415,17 @@
       </c>
       <c r="D143" s="9"/>
       <c r="E143" s="5"/>
-      <c r="F143" s="9"/>
+      <c r="F143" s="9">
+        <v>9</v>
+      </c>
       <c r="G143" s="9"/>
       <c r="H143" s="6"/>
-      <c r="I143" s="6"/>
-      <c r="J143" s="6"/>
+      <c r="I143" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J143" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
@@ -21343,11 +21439,17 @@
       </c>
       <c r="D144" s="9"/>
       <c r="E144" s="5"/>
-      <c r="F144" s="9"/>
+      <c r="F144" s="9">
+        <v>4</v>
+      </c>
       <c r="G144" s="9"/>
       <c r="H144" s="6"/>
-      <c r="I144" s="6"/>
-      <c r="J144" s="6"/>
+      <c r="I144" s="30" t="s">
+        <v>832</v>
+      </c>
+      <c r="J144" s="30" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">

</xml_diff>